<commit_message>
Check if valid template or not
</commit_message>
<xml_diff>
--- a/WebApplication5/Staff_Details.xlsx
+++ b/WebApplication5/Staff_Details.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohit\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohit\source\repos\WebApplication5\WebApplication5\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -38,60 +38,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
-  <si>
-    <t>Staff_Name</t>
-  </si>
-  <si>
-    <t>Staff_Id</t>
-  </si>
-  <si>
-    <t>Staff_Type</t>
-  </si>
-  <si>
-    <t>Staff_Address</t>
-  </si>
-  <si>
-    <t>Staff_ZipCode</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>peter</t>
   </si>
   <si>
-    <t>head master</t>
-  </si>
-  <si>
     <t>tell drive, tx</t>
   </si>
   <si>
     <t>mary</t>
   </si>
   <si>
-    <t>science teacher</t>
-  </si>
-  <si>
     <t>mcneil drive, tx</t>
   </si>
   <si>
     <t>yao</t>
   </si>
   <si>
-    <t>maths teacher</t>
-  </si>
-  <si>
     <t>keeper drive, tx</t>
   </si>
   <si>
     <t>umran</t>
   </si>
   <si>
-    <t>PET</t>
-  </si>
-  <si>
     <t>irish drive, tx</t>
   </si>
   <si>
     <t>Evaluation Only. Created with Aspose.Cells for .NET.Copyright 2003 - 2023 Aspose Pty Ltd.</t>
+  </si>
+  <si>
+    <t>Student_Name</t>
+  </si>
+  <si>
+    <t>Student_Id</t>
+  </si>
+  <si>
+    <t>Student_Grade</t>
+  </si>
+  <si>
+    <t>Student_Address</t>
+  </si>
+  <si>
+    <t>Student_ZipCode</t>
   </si>
 </sst>
 </file>
@@ -165,10 +153,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment/>
-      <protection/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment/>
       <protection/>
@@ -562,47 +547,47 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
-      <selection pane="topLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="topLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11.285714285714286" customWidth="1"/>
+    <col min="1" max="1" width="13.285714285714286" customWidth="1"/>
     <col min="2" max="2" width="11.428571428571429" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="11.714285714285714" customWidth="1"/>
+    <col min="4" max="4" width="14.857142857142858" customWidth="1"/>
+    <col min="5" max="5" width="14.285714285714286" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.4">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.4">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>45</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
+      <c r="C2">
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>79415</v>
@@ -610,16 +595,16 @@
     </row>
     <row r="3" spans="1:5" ht="14.4">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>54</v>
       </c>
-      <c r="C3" t="s">
-        <v>9</v>
+      <c r="C3">
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E3">
         <v>79416</v>
@@ -627,16 +612,16 @@
     </row>
     <row r="4" spans="1:5" ht="14.4">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>89</v>
       </c>
-      <c r="C4" t="s">
-        <v>12</v>
+      <c r="C4">
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="E4">
         <v>79876</v>
@@ -644,16 +629,16 @@
     </row>
     <row r="5" spans="1:5" ht="14.4">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>90</v>
       </c>
-      <c r="C5" t="s">
-        <v>15</v>
+      <c r="C5">
+        <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E5">
         <v>78562</v>
@@ -665,16 +650,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ef7f2f68-e6c7-4ea3-b802-cc40fae7c4e4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8628E9C9-CB6F-462F-AF17-8CB814CD9BB1}">
   <dimension ref="A5"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="5" spans="1:1" ht="23.25" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -683,7 +668,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1dc33522-e390-4bfa-ae67-dc05aabab78c}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78cedd58-fa8c-4010-844c-beda8356bf2d}">
   <dimension ref="A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1"/>
@@ -692,7 +677,7 @@
   <sheetData>
     <row r="5" spans="1:1" ht="23.25" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>